<commit_message>
Updated the Install.md for updates. Added additional evidences.
</commit_message>
<xml_diff>
--- a/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
+++ b/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -149,9 +149,6 @@
 b_GSA-ADS-FDA-Prototype_ProjectPlan-AceInfo.pdf</t>
   </si>
   <si>
-    <t>e_GSA-ADS-FDA-Prototype_StyleGuide-AceInfo.pdf</t>
-  </si>
-  <si>
     <t>f_GSA-ADS-FDA-Prototype_UsabilityTests-AceInfo.jpg
 f_GSA-ADS-FDA-Prototype_UsabilityTestsEmail-AceInfo.pdf</t>
   </si>
@@ -170,17 +167,10 @@
     <t>h_GSA-ADS-FDA-Prototype_MultipleDevices_Android_iOS-AceInfo.pdf</t>
   </si>
   <si>
-    <t>Ruby on Rails, HTML 5, Twitter Bootstrap, ChartKick, JIRA, Git, Selenium, Jmeter, Jenkins and Docker.
-i_GSA-ADS-FDA-Prototype_TechnicalArchitectureDiagram-AceInfo.pdf</t>
-  </si>
-  <si>
     <t>j_GSA-ADS-FDA-Prototype_PaaS_AWScloud-AceInfo.pdf</t>
   </si>
   <si>
     <t>l_GSA-ADS-FDA-Prototype_ContinuousIntegrationSystem-AceInfo.pdf</t>
-  </si>
-  <si>
-    <t>k_GSA-ADS-FDA-Prototype_AutomatedUnitTestResults-AceInfo.pdf</t>
   </si>
   <si>
     <t>m_GSA-ADS-DA-Prototype_ConfigurationManagement-AceInfo.pdf</t>
@@ -209,12 +199,30 @@
 g_GSA-ADS-BPA-FDAPrototype_GUIDesigns_v3-AceInfo.zip
 g_GSA-ADS-BPA-FDAPrototype_GUIDesigns_v4-AceInfo.zip</t>
   </si>
+  <si>
+    <t>k_GSA-ADS-FDA-Prototype_AutomatedUnitTestResults-AceInfo.pdf
+k_GSA-ADS-FDA-Prototype_JMeterLoadTesting-AceInfo.pdf
+k_GSA-ADS-FDA-Prototype_Section508_Testing-AceInfo.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e_GSA-ADS-FDA-Prototype_StyleGuide-AceInfo.pdf
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_GSA-ADS-FDA-Prototype_Kickoff-TeamRoles-AceInfo.pdf
+a_GSA-ADS-FDA-Prototype_Kickoff-AceInfo.jpg
+</t>
+  </si>
+  <si>
+    <t>Ruby on Rails, HTML 5, Twitter Bootstrap, ChartKick, JIRA, Git, Selenium, Jmeter, Jenkins and Docker.
+i_GSA-ADS-FDA-Prototype_TechnicalArchitectureDiagram-AceInfo.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -236,6 +244,13 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,10 +285,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -284,8 +300,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -10856,15 +10876,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="78.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.7109375" style="3" customWidth="1"/>
     <col min="4" max="26" width="14.42578125" style="3" customWidth="1"/>
     <col min="27" max="16384" width="17.28515625" style="3"/>
   </cols>
@@ -10883,7 +10903,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -10891,9 +10911,9 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
@@ -10919,7 +10939,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -10933,7 +10953,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -10947,7 +10967,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -10961,13 +10981,13 @@
         <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -10975,7 +10995,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -10989,13 +11009,13 @@
         <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -11003,7 +11023,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -11017,13 +11037,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -11031,7 +11051,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -11045,7 +11065,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -11059,13 +11079,13 @@
         <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" s="5" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="5" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -11073,7 +11093,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -11087,7 +11107,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -11101,13 +11121,13 @@
         <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
@@ -11115,7 +11135,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -11129,7 +11149,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>

</xml_diff>

<commit_message>
renamed a file in the evidences column
</commit_message>
<xml_diff>
--- a/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
+++ b/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATummala\Desktop\GSAADSBPA-FDAPrototype\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19440" windowHeight="7035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="design pool evidence" sheetId="1" r:id="rId1"/>
@@ -173,9 +178,6 @@
     <t>l_GSA-ADS-FDA-Prototype_ContinuousIntegrationSystem-AceInfo.pdf</t>
   </si>
   <si>
-    <t>m_GSA-ADS-DA-Prototype_ConfigurationManagement-AceInfo.pdf</t>
-  </si>
-  <si>
     <t>o_GSA-ADS-FDA-Prototype_DockerContainer-AceInfo.pdf</t>
   </si>
   <si>
@@ -216,6 +218,9 @@
   <si>
     <t>Ruby on Rails, HTML 5, Twitter Bootstrap, ChartKick, Git, Selenium, Jmeter, Jenkins and Docker.
 i_GSA-ADS-FDA-Prototype_TechnicalArchitectureDiagram-AceInfo.pdf</t>
+  </si>
+  <si>
+    <t>m_GSA-ADS-FDA-Prototype_ConfigurationManagement-AceInfo.pdf</t>
   </si>
 </sst>
 </file>
@@ -364,7 +369,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,7 +404,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10876,7 +10881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10909,7 +10916,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="2"/>
@@ -10965,7 +10972,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -10993,7 +11000,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -11021,7 +11028,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -11049,7 +11056,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -11077,7 +11084,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -11091,7 +11098,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -11105,7 +11112,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -11119,7 +11126,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -11133,7 +11140,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>

</xml_diff>